<commit_message>
Update The federal learning part
</commit_message>
<xml_diff>
--- a/data/hotpot_screen_data.xlsx
+++ b/data/hotpot_screen_data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xueti\Dropbox (University of Michigan)\Umich\class\term2\620\bios620_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72B8129-A17A-4CC5-A680-747D8D88C15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83B1F46-6B6E-4C25-A464-8CE9E93077B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{18B1CDC2-9177-7E47-AC91-4E14230D10A6}"/>
+    <workbookView xWindow="5280" yWindow="480" windowWidth="13680" windowHeight="11340" activeTab="2" xr2:uid="{18B1CDC2-9177-7E47-AC91-4E14230D10A6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overall" sheetId="1" r:id="rId1"/>
+    <sheet name="xuetao" sheetId="2" r:id="rId2"/>
+    <sheet name="isgomez" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -50,9 +52,6 @@
   </si>
   <si>
     <t>Pickups</t>
-  </si>
-  <si>
-    <t>1st.Pickup</t>
   </si>
   <si>
     <t>Team</t>
@@ -89,6 +88,9 @@
   </si>
   <si>
     <t>xuetao</t>
+  </si>
+  <si>
+    <t>Pickup.1st</t>
   </si>
 </sst>
 </file>
@@ -445,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98575874-61FD-7241-92FB-663E99FFADF0}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="101" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -461,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -476,21 +478,21 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>44564</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>116</v>
@@ -505,18 +507,18 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>44565</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>89</v>
@@ -531,18 +533,18 @@
         <v>0.41388888888888892</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>44566</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>354</v>
@@ -557,18 +559,18 @@
         <v>0.24791666666666667</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>44567</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>414</v>
@@ -583,18 +585,18 @@
         <v>0.40208333333333335</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>44568</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>283</v>
@@ -609,18 +611,18 @@
         <v>0.33194444444444443</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>44569</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>219</v>
@@ -635,18 +637,18 @@
         <v>0.42291666666666666</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>44570</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>369</v>
@@ -661,18 +663,18 @@
         <v>0.28541666666666665</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>44571</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>283</v>
@@ -687,18 +689,18 @@
         <v>0.27777777777777779</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>44572</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>364</v>
@@ -713,18 +715,18 @@
         <v>0.48125000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>44573</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>352</v>
@@ -739,18 +741,18 @@
         <v>0.41250000000000003</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
         <v>44574</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>316</v>
@@ -765,18 +767,18 @@
         <v>0.26180555555555557</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>44575</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>221</v>
@@ -791,18 +793,18 @@
         <v>0.25208333333333333</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>44576</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>644</v>
@@ -817,18 +819,18 @@
         <v>0.22777777777777777</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>44577</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <v>264</v>
@@ -843,18 +845,18 @@
         <v>0.52638888888888891</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>44578</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16">
         <v>644</v>
@@ -869,18 +871,18 @@
         <v>0.36805555555555558</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>44579</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>256</v>
@@ -895,18 +897,18 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
         <v>44580</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>490</v>
@@ -921,18 +923,18 @@
         <v>0.36805555555555558</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
         <v>44581</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>328</v>
@@ -947,18 +949,18 @@
         <v>0.46319444444444446</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
         <v>44582</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <v>460</v>
@@ -973,18 +975,18 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1">
         <v>44583</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>340</v>
@@ -999,18 +1001,18 @@
         <v>0.4458333333333333</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1">
         <v>44584</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>615</v>
@@ -1025,18 +1027,18 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="H22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
         <v>44575</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23">
         <f>11*60+41</f>
@@ -1052,18 +1054,18 @@
         <v>0.31111111111111112</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1">
         <v>44576</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <f>9*60+34</f>
@@ -1080,18 +1082,18 @@
         <v>0.34722222222222227</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1">
         <v>44577</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25">
         <f>11*60+2</f>
@@ -1107,18 +1109,18 @@
         <v>0.3125</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1">
         <v>44578</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26">
         <f>10*60+52</f>
@@ -1134,18 +1136,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1">
         <v>44579</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <f>10*60+2</f>
@@ -1161,18 +1163,18 @@
         <v>0.28125</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1">
         <v>44580</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <f>9*60+39</f>
@@ -1188,18 +1190,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1">
         <v>44581</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <f>5*60+26</f>
@@ -1215,18 +1217,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1">
         <v>44582</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30">
         <f>4*60+13</f>
@@ -1242,18 +1244,18 @@
         <v>0.34375</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="1">
         <v>44583</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <f>2*60+7</f>
@@ -1269,18 +1271,18 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="H31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="1">
         <v>44584</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32">
         <f>13*60+8</f>
@@ -1296,18 +1298,18 @@
         <v>0.28333333333333333</v>
       </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="1">
         <v>44585</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33">
         <f>8*60+4</f>
@@ -1323,18 +1325,18 @@
         <v>0.2722222222222222</v>
       </c>
       <c r="H33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1">
         <v>44586</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34">
         <f>4*60+25</f>
@@ -1350,18 +1352,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1">
         <v>44587</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35">
         <f>9*60+3</f>
@@ -1378,18 +1380,18 @@
         <v>0.27916666666666667</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" s="1">
         <v>44588</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36">
         <f>11*60+16</f>
@@ -1406,18 +1408,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="1">
         <v>44589</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D37">
         <f>5*60+54</f>
@@ -1433,18 +1435,18 @@
         <v>0.30833333333333335</v>
       </c>
       <c r="H37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" s="1">
         <v>44590</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38">
         <f>9*60+22</f>
@@ -1461,18 +1463,18 @@
         <v>0.23263888888888887</v>
       </c>
       <c r="H38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" s="1">
         <v>44591</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D39">
         <f>9*60+51</f>
@@ -1489,18 +1491,18 @@
         <v>0.32430555555555557</v>
       </c>
       <c r="H39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" s="1">
         <v>44592</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D40">
         <f>10*60+37</f>
@@ -1517,18 +1519,18 @@
         <v>0.28611111111111115</v>
       </c>
       <c r="H40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="1">
         <v>44593</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41">
         <v>327</v>
@@ -1543,18 +1545,18 @@
         <v>0.28263888888888888</v>
       </c>
       <c r="H41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42" s="1">
         <v>44594</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42">
         <f>7*60+51</f>
@@ -1570,18 +1572,18 @@
         <v>0.27986111111111112</v>
       </c>
       <c r="H42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="1">
         <v>44595</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43">
         <f>6*60+48</f>
@@ -1597,18 +1599,18 @@
         <v>0.28263888888888888</v>
       </c>
       <c r="H43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44" s="1">
         <v>44596</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D44">
         <f>4*60+16</f>
@@ -1624,18 +1626,18 @@
         <v>0.31736111111111115</v>
       </c>
       <c r="H44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="1">
         <v>44597</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45">
         <f>4*60+15</f>
@@ -1651,18 +1653,18 @@
         <v>0.28472222222222221</v>
       </c>
       <c r="H45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B46" s="1">
         <v>44598</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46">
         <v>158</v>
@@ -1677,18 +1679,18 @@
         <v>0.32916666666666666</v>
       </c>
       <c r="H46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="1">
         <v>44599</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D47">
         <v>207</v>
@@ -1703,18 +1705,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B48" s="1">
         <v>44600</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D48">
         <v>581</v>
@@ -1729,18 +1731,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B49" s="1">
         <v>44601</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D49">
         <v>650</v>
@@ -1755,18 +1757,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B50" s="1">
         <v>44602</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50">
         <v>342</v>
@@ -1781,18 +1783,18 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="H50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B51" s="1">
         <v>44603</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D51">
         <v>449</v>
@@ -1807,18 +1809,18 @@
         <v>0.30694444444444441</v>
       </c>
       <c r="H51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" s="1">
         <v>44604</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D52">
         <v>497</v>
@@ -1833,18 +1835,18 @@
         <v>0.31597222222222221</v>
       </c>
       <c r="H52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B53" s="1">
         <v>44605</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D53">
         <v>343</v>
@@ -1859,7 +1861,1472 @@
         <v>0.30902777777777779</v>
       </c>
       <c r="H53" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D74119D-B011-4856-A6BF-B41B3D0737F9}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44575</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <f>11*60+41</f>
+        <v>701</v>
+      </c>
+      <c r="E2">
+        <v>52</v>
+      </c>
+      <c r="F2">
+        <v>52</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44576</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <f>9*60+34</f>
+        <v>574</v>
+      </c>
+      <c r="E3">
+        <f>2*60+27</f>
+        <v>147</v>
+      </c>
+      <c r="F3">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44577</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <f>11*60+2</f>
+        <v>662</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44578</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <f>10*60+52</f>
+        <v>652</v>
+      </c>
+      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44579</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f>10*60+2</f>
+        <v>602</v>
+      </c>
+      <c r="E6">
+        <v>49</v>
+      </c>
+      <c r="F6">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.28125</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44580</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <f>9*60+39</f>
+        <v>579</v>
+      </c>
+      <c r="E7">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44581</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <f>5*60+26</f>
+        <v>326</v>
+      </c>
+      <c r="E8">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>31</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44582</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <f>4*60+13</f>
+        <v>253</v>
+      </c>
+      <c r="E9">
+        <v>53</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44583</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <f>2*60+7</f>
+        <v>127</v>
+      </c>
+      <c r="E10">
+        <v>51</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44584</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <f>13*60+8</f>
+        <v>788</v>
+      </c>
+      <c r="E11">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44585</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <f>8*60+4</f>
+        <v>484</v>
+      </c>
+      <c r="E12">
+        <v>70</v>
+      </c>
+      <c r="F12">
+        <v>42</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.2722222222222222</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44586</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <f>4*60+25</f>
+        <v>265</v>
+      </c>
+      <c r="E13">
+        <v>64</v>
+      </c>
+      <c r="F13">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44587</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <f>9*60+3</f>
+        <v>543</v>
+      </c>
+      <c r="E14">
+        <f>83</f>
+        <v>83</v>
+      </c>
+      <c r="F14">
+        <v>35</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.27916666666666667</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44588</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <f>11*60+16</f>
+        <v>676</v>
+      </c>
+      <c r="E15">
+        <f>2*60+26</f>
+        <v>146</v>
+      </c>
+      <c r="F15">
+        <v>32</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44589</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f>5*60+54</f>
+        <v>354</v>
+      </c>
+      <c r="E16">
+        <v>33</v>
+      </c>
+      <c r="F16">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.30833333333333335</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44590</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <f>9*60+22</f>
+        <v>562</v>
+      </c>
+      <c r="E17">
+        <f>1*60+8</f>
+        <v>68</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.23263888888888887</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44591</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <f>9*60+51</f>
+        <v>591</v>
+      </c>
+      <c r="E18">
+        <f>2*60+38</f>
+        <v>158</v>
+      </c>
+      <c r="F18">
+        <v>22</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.32430555555555557</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44592</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <f>10*60+37</f>
+        <v>637</v>
+      </c>
+      <c r="E19">
+        <f>3*60+8</f>
+        <v>188</v>
+      </c>
+      <c r="F19">
+        <v>60</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.28611111111111115</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44593</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>327</v>
+      </c>
+      <c r="E20">
+        <v>280</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.28263888888888888</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44594</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <f>7*60+51</f>
+        <v>471</v>
+      </c>
+      <c r="E21">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>22</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44595</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <f>6*60+48</f>
+        <v>408</v>
+      </c>
+      <c r="E22">
+        <v>54</v>
+      </c>
+      <c r="F22">
+        <v>28</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.28263888888888888</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44596</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <f>4*60+16</f>
+        <v>256</v>
+      </c>
+      <c r="E23">
+        <v>94</v>
+      </c>
+      <c r="F23">
+        <v>16</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44597</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <f>4*60+15</f>
+        <v>255</v>
+      </c>
+      <c r="E24">
+        <v>123</v>
+      </c>
+      <c r="F24">
+        <v>19</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.28472222222222221</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44598</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>158</v>
+      </c>
+      <c r="E25">
+        <v>85</v>
+      </c>
+      <c r="F25">
+        <v>16</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.32916666666666666</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44599</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>207</v>
+      </c>
+      <c r="E26">
+        <v>93</v>
+      </c>
+      <c r="F26">
+        <v>32</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44600</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>581</v>
+      </c>
+      <c r="E27">
+        <v>68</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44601</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>650</v>
+      </c>
+      <c r="E28">
+        <v>43</v>
+      </c>
+      <c r="F28">
+        <v>41</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44602</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>342</v>
+      </c>
+      <c r="E29">
+        <v>94</v>
+      </c>
+      <c r="F29">
+        <v>48</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44603</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>449</v>
+      </c>
+      <c r="E30">
+        <v>212</v>
+      </c>
+      <c r="F30">
+        <v>24</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.30694444444444441</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44604</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>497</v>
+      </c>
+      <c r="E31">
+        <v>12</v>
+      </c>
+      <c r="F31">
+        <v>28</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44605</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>343</v>
+      </c>
+      <c r="E32">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>38</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B966CB-B398-460C-B036-F264240E34D4}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44564</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>116</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>118</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44565</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>89</v>
+      </c>
+      <c r="E3">
+        <v>49</v>
+      </c>
+      <c r="F3">
+        <v>101</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.41388888888888892</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44566</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>354</v>
+      </c>
+      <c r="E4">
+        <v>233</v>
+      </c>
+      <c r="F4">
+        <v>126</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.24791666666666667</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44567</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>414</v>
+      </c>
+      <c r="E5">
+        <v>258</v>
+      </c>
+      <c r="F5">
+        <v>128</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.40208333333333335</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44568</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>283</v>
+      </c>
+      <c r="E6">
+        <v>189</v>
+      </c>
+      <c r="F6">
+        <v>147</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.33194444444444443</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44569</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>219</v>
+      </c>
+      <c r="E7">
+        <v>84</v>
+      </c>
+      <c r="F7">
+        <v>161</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44570</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>369</v>
+      </c>
+      <c r="E8">
+        <v>87</v>
+      </c>
+      <c r="F8">
+        <v>205</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.28541666666666665</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44571</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>283</v>
+      </c>
+      <c r="E9">
+        <v>109</v>
+      </c>
+      <c r="F9">
+        <v>166</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44572</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>364</v>
+      </c>
+      <c r="E10">
+        <v>129</v>
+      </c>
+      <c r="F10">
+        <v>97</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44573</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>352</v>
+      </c>
+      <c r="E11">
+        <v>174</v>
+      </c>
+      <c r="F11">
+        <v>112</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.41250000000000003</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44574</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>316</v>
+      </c>
+      <c r="E12">
+        <v>192</v>
+      </c>
+      <c r="F12">
+        <v>151</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.26180555555555557</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44575</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>221</v>
+      </c>
+      <c r="E13">
+        <v>81</v>
+      </c>
+      <c r="F13">
+        <v>176</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.25208333333333333</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44576</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>644</v>
+      </c>
+      <c r="E14">
+        <v>317</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.22777777777777777</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44577</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>264</v>
+      </c>
+      <c r="E15">
+        <v>66</v>
+      </c>
+      <c r="F15">
+        <v>97</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44578</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>644</v>
+      </c>
+      <c r="E16">
+        <v>79</v>
+      </c>
+      <c r="F16">
+        <v>97</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44579</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>256</v>
+      </c>
+      <c r="E17">
+        <v>119</v>
+      </c>
+      <c r="F17">
+        <v>72</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44580</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>490</v>
+      </c>
+      <c r="E18">
+        <v>214</v>
+      </c>
+      <c r="F18">
+        <v>126</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44581</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>328</v>
+      </c>
+      <c r="E19">
+        <v>108</v>
+      </c>
+      <c r="F19">
+        <v>120</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44582</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>460</v>
+      </c>
+      <c r="E20">
+        <v>136</v>
+      </c>
+      <c r="F20">
+        <v>150</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44583</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>340</v>
+      </c>
+      <c r="E21">
+        <v>77</v>
+      </c>
+      <c r="F21">
+        <v>128</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.4458333333333333</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44584</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>615</v>
+      </c>
+      <c r="E22">
+        <v>206</v>
+      </c>
+      <c r="F22">
+        <v>153</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating screen data for isabel
</commit_message>
<xml_diff>
--- a/data/hotpot_screen_data.xlsx
+++ b/data/hotpot_screen_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xueti\Dropbox (University of Michigan)\Umich\class\term2\620\bios620_project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igome\Documents\UMich\Winter 2022\620\bios620_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72B8129-A17A-4CC5-A680-747D8D88C15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C846995-F320-440B-AF37-DBDB472A3AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{18B1CDC2-9177-7E47-AC91-4E14230D10A6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{18B1CDC2-9177-7E47-AC91-4E14230D10A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -443,20 +442,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98575874-61FD-7241-92FB-663E99FFADF0}">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="101" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.3125" customWidth="1"/>
-    <col min="5" max="5" width="12.8125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -508,7 +507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -534,7 +533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -560,7 +559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -586,7 +585,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -612,7 +611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -638,7 +637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -664,7 +663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -690,7 +689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -716,7 +715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -742,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -768,7 +767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -794,7 +793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -820,7 +819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -846,7 +845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -872,7 +871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -898,7 +897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -924,7 +923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -950,7 +949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -976,7 +975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1002,7 +1001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1028,837 +1027,1311 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
+        <v>44585</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44586</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44587</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44588</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44589</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44590</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44591</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>372</v>
+      </c>
+      <c r="E29">
+        <v>141</v>
+      </c>
+      <c r="F29">
+        <v>161</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.46597222222222223</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44592</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>332</v>
+      </c>
+      <c r="E30">
+        <v>47</v>
+      </c>
+      <c r="F30">
+        <v>157</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44593</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>342</v>
+      </c>
+      <c r="E31">
+        <v>91</v>
+      </c>
+      <c r="F31">
+        <v>308</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.24930555555555556</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44594</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>405</v>
+      </c>
+      <c r="E32">
+        <v>230</v>
+      </c>
+      <c r="F32">
+        <v>172</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44595</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>250</v>
+      </c>
+      <c r="E33">
+        <v>83</v>
+      </c>
+      <c r="F33">
+        <v>219</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44596</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>212</v>
+      </c>
+      <c r="E34">
+        <v>44</v>
+      </c>
+      <c r="F34">
+        <v>227</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44597</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>276</v>
+      </c>
+      <c r="E35">
+        <v>62</v>
+      </c>
+      <c r="F35">
+        <v>331</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44598</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36">
+        <v>439</v>
+      </c>
+      <c r="E36">
+        <v>56</v>
+      </c>
+      <c r="F36">
+        <v>219</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44599</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>535</v>
+      </c>
+      <c r="E37">
+        <v>113</v>
+      </c>
+      <c r="F37">
+        <v>156</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.21597222222222223</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44600</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38">
+        <v>532</v>
+      </c>
+      <c r="E38">
+        <v>189</v>
+      </c>
+      <c r="F38">
+        <v>155</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1">
+        <v>44601</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39">
+        <v>259</v>
+      </c>
+      <c r="E39">
+        <v>148</v>
+      </c>
+      <c r="F39">
+        <v>181</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.31527777777777777</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44602</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40">
+        <v>340</v>
+      </c>
+      <c r="E40">
+        <v>123</v>
+      </c>
+      <c r="F40">
+        <v>176</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44603</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>411</v>
+      </c>
+      <c r="E41">
+        <v>216</v>
+      </c>
+      <c r="F41">
+        <v>163</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.33958333333333335</v>
+      </c>
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44604</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>516</v>
+      </c>
+      <c r="E42">
+        <v>95</v>
+      </c>
+      <c r="F42">
+        <v>188</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44605</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>501</v>
+      </c>
+      <c r="E43">
+        <v>89</v>
+      </c>
+      <c r="F43">
+        <v>172</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.33958333333333335</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="1">
         <v>44575</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D23">
+      <c r="D44">
         <f>11*60+41</f>
         <v>701</v>
       </c>
-      <c r="E23">
+      <c r="E44">
         <v>52</v>
       </c>
-      <c r="F23">
+      <c r="F44">
         <v>52</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G44" s="2">
         <v>0.31111111111111112</v>
       </c>
-      <c r="H23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="1">
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="1">
         <v>44576</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C45" t="s">
         <v>8</v>
       </c>
-      <c r="D24">
+      <c r="D45">
         <f>9*60+34</f>
         <v>574</v>
       </c>
-      <c r="E24">
+      <c r="E45">
         <f>2*60+27</f>
         <v>147</v>
       </c>
-      <c r="F24">
+      <c r="F45">
         <v>19</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G45" s="2">
         <v>0.34722222222222227</v>
       </c>
-      <c r="H24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="1">
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="1">
         <v>44577</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C46" t="s">
         <v>9</v>
       </c>
-      <c r="D25">
+      <c r="D46">
         <f>11*60+2</f>
         <v>662</v>
       </c>
-      <c r="E25">
+      <c r="E46">
         <v>12</v>
       </c>
-      <c r="F25">
+      <c r="F46">
         <v>21</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G46" s="2">
         <v>0.3125</v>
       </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="1">
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1">
         <v>44578</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C47" t="s">
         <v>10</v>
       </c>
-      <c r="D26">
+      <c r="D47">
         <f>10*60+52</f>
         <v>652</v>
       </c>
-      <c r="E26">
+      <c r="E47">
         <v>22</v>
       </c>
-      <c r="F26">
+      <c r="F47">
         <v>26</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G47" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="1">
+      <c r="H47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="1">
         <v>44579</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C48" t="s">
         <v>11</v>
       </c>
-      <c r="D27">
+      <c r="D48">
         <f>10*60+2</f>
         <v>602</v>
       </c>
-      <c r="E27">
+      <c r="E48">
         <v>49</v>
       </c>
-      <c r="F27">
+      <c r="F48">
         <v>24</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G48" s="2">
         <v>0.28125</v>
       </c>
-      <c r="H27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="1">
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="1">
         <v>44580</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C49" t="s">
         <v>12</v>
       </c>
-      <c r="D28">
+      <c r="D49">
         <f>9*60+39</f>
         <v>579</v>
       </c>
-      <c r="E28">
+      <c r="E49">
         <v>19</v>
       </c>
-      <c r="F28">
+      <c r="F49">
         <v>24</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G49" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="1">
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" s="1">
         <v>44581</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C50" t="s">
         <v>13</v>
       </c>
-      <c r="D29">
+      <c r="D50">
         <f>5*60+26</f>
         <v>326</v>
       </c>
-      <c r="E29">
+      <c r="E50">
         <v>28</v>
       </c>
-      <c r="F29">
+      <c r="F50">
         <v>31</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G50" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="1">
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="1">
         <v>44582</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C51" t="s">
         <v>7</v>
       </c>
-      <c r="D30">
+      <c r="D51">
         <f>4*60+13</f>
         <v>253</v>
       </c>
-      <c r="E30">
+      <c r="E51">
         <v>53</v>
       </c>
-      <c r="F30">
+      <c r="F51">
         <v>28</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G51" s="2">
         <v>0.34375</v>
       </c>
-      <c r="H30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="1">
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="1">
         <v>44583</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C52" t="s">
         <v>8</v>
       </c>
-      <c r="D31">
+      <c r="D52">
         <f>2*60+7</f>
         <v>127</v>
       </c>
-      <c r="E31">
+      <c r="E52">
         <v>51</v>
       </c>
-      <c r="F31">
-        <v>15</v>
-      </c>
-      <c r="G31" s="2">
+      <c r="F52">
+        <v>15</v>
+      </c>
+      <c r="G52" s="2">
         <v>0.35416666666666669</v>
       </c>
-      <c r="H31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="1">
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1">
         <v>44584</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C53" t="s">
         <v>9</v>
       </c>
-      <c r="D32">
+      <c r="D53">
         <f>13*60+8</f>
         <v>788</v>
       </c>
-      <c r="E32">
+      <c r="E53">
         <v>31</v>
       </c>
-      <c r="F32">
+      <c r="F53">
         <v>22</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G53" s="2">
         <v>0.28333333333333333</v>
       </c>
-      <c r="H32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="1">
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="1">
         <v>44585</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C54" t="s">
         <v>10</v>
       </c>
-      <c r="D33">
+      <c r="D54">
         <f>8*60+4</f>
         <v>484</v>
       </c>
-      <c r="E33">
+      <c r="E54">
         <v>70</v>
       </c>
-      <c r="F33">
+      <c r="F54">
         <v>42</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G54" s="2">
         <v>0.2722222222222222</v>
       </c>
-      <c r="H33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="1">
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="1">
         <v>44586</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C55" t="s">
         <v>11</v>
       </c>
-      <c r="D34">
+      <c r="D55">
         <f>4*60+25</f>
         <v>265</v>
       </c>
-      <c r="E34">
+      <c r="E55">
         <v>64</v>
       </c>
-      <c r="F34">
+      <c r="F55">
         <v>39</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G55" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A35" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="1">
+      <c r="H55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="1">
         <v>44587</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C56" t="s">
         <v>12</v>
       </c>
-      <c r="D35">
+      <c r="D56">
         <f>9*60+3</f>
         <v>543</v>
       </c>
-      <c r="E35">
+      <c r="E56">
         <f>83</f>
         <v>83</v>
       </c>
-      <c r="F35">
+      <c r="F56">
         <v>35</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G56" s="2">
         <v>0.27916666666666667</v>
       </c>
-      <c r="H35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="1">
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="1">
         <v>44588</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C57" t="s">
         <v>13</v>
       </c>
-      <c r="D36">
+      <c r="D57">
         <f>11*60+16</f>
         <v>676</v>
       </c>
-      <c r="E36">
+      <c r="E57">
         <f>2*60+26</f>
         <v>146</v>
       </c>
-      <c r="F36">
+      <c r="F57">
         <v>32</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G57" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="1">
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="1">
         <v>44589</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C58" t="s">
         <v>7</v>
       </c>
-      <c r="D37">
+      <c r="D58">
         <f>5*60+54</f>
         <v>354</v>
       </c>
-      <c r="E37">
+      <c r="E58">
         <v>33</v>
       </c>
-      <c r="F37">
+      <c r="F58">
         <v>34</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G58" s="2">
         <v>0.30833333333333335</v>
       </c>
-      <c r="H37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="1">
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="1">
         <v>44590</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C59" t="s">
         <v>8</v>
       </c>
-      <c r="D38">
+      <c r="D59">
         <f>9*60+22</f>
         <v>562</v>
       </c>
-      <c r="E38">
+      <c r="E59">
         <f>1*60+8</f>
         <v>68</v>
       </c>
-      <c r="F38">
+      <c r="F59">
         <v>14</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G59" s="2">
         <v>0.23263888888888887</v>
       </c>
-      <c r="H38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A39" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="1">
+      <c r="H59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="1">
         <v>44591</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C60" t="s">
         <v>9</v>
       </c>
-      <c r="D39">
+      <c r="D60">
         <f>9*60+51</f>
         <v>591</v>
       </c>
-      <c r="E39">
+      <c r="E60">
         <f>2*60+38</f>
         <v>158</v>
       </c>
-      <c r="F39">
+      <c r="F60">
         <v>22</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G60" s="2">
         <v>0.32430555555555557</v>
       </c>
-      <c r="H39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A40" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="1">
+      <c r="H60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" s="1">
         <v>44592</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C61" t="s">
         <v>10</v>
       </c>
-      <c r="D40">
+      <c r="D61">
         <f>10*60+37</f>
         <v>637</v>
       </c>
-      <c r="E40">
+      <c r="E61">
         <f>3*60+8</f>
         <v>188</v>
       </c>
-      <c r="F40">
+      <c r="F61">
         <v>60</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G61" s="2">
         <v>0.28611111111111115</v>
       </c>
-      <c r="H40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="1">
+      <c r="H61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="1">
         <v>44593</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C62" t="s">
         <v>11</v>
       </c>
-      <c r="D41">
+      <c r="D62">
         <v>327</v>
       </c>
-      <c r="E41">
+      <c r="E62">
         <v>280</v>
       </c>
-      <c r="F41">
+      <c r="F62">
         <v>60</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G62" s="2">
         <v>0.28263888888888888</v>
       </c>
-      <c r="H41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="1">
+      <c r="H62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="1">
         <v>44594</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C63" t="s">
         <v>12</v>
       </c>
-      <c r="D42">
+      <c r="D63">
         <f>7*60+51</f>
         <v>471</v>
       </c>
-      <c r="E42">
+      <c r="E63">
         <v>80</v>
       </c>
-      <c r="F42">
+      <c r="F63">
         <v>22</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G63" s="2">
         <v>0.27986111111111112</v>
       </c>
-      <c r="H42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A43" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="1">
+      <c r="H63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" s="1">
         <v>44595</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C64" t="s">
         <v>13</v>
       </c>
-      <c r="D43">
+      <c r="D64">
         <f>6*60+48</f>
         <v>408</v>
       </c>
-      <c r="E43">
+      <c r="E64">
         <v>54</v>
       </c>
-      <c r="F43">
+      <c r="F64">
         <v>28</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G64" s="2">
         <v>0.28263888888888888</v>
       </c>
-      <c r="H43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" s="1">
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="1">
         <v>44596</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C65" t="s">
         <v>7</v>
       </c>
-      <c r="D44">
+      <c r="D65">
         <f>4*60+16</f>
         <v>256</v>
       </c>
-      <c r="E44">
+      <c r="E65">
         <v>94</v>
       </c>
-      <c r="F44">
-        <v>16</v>
-      </c>
-      <c r="G44" s="2">
+      <c r="F65">
+        <v>16</v>
+      </c>
+      <c r="G65" s="2">
         <v>0.31736111111111115</v>
       </c>
-      <c r="H44" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="1">
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" s="1">
         <v>44597</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C66" t="s">
         <v>8</v>
       </c>
-      <c r="D45">
+      <c r="D66">
         <f>4*60+15</f>
         <v>255</v>
       </c>
-      <c r="E45">
+      <c r="E66">
         <v>123</v>
       </c>
-      <c r="F45">
+      <c r="F66">
         <v>19</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G66" s="2">
         <v>0.28472222222222221</v>
       </c>
-      <c r="H45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A46" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="1">
+      <c r="H66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="1">
         <v>44598</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C67" t="s">
         <v>9</v>
       </c>
-      <c r="D46">
+      <c r="D67">
         <v>158</v>
       </c>
-      <c r="E46">
+      <c r="E67">
         <v>85</v>
       </c>
-      <c r="F46">
-        <v>16</v>
-      </c>
-      <c r="G46" s="2">
+      <c r="F67">
+        <v>16</v>
+      </c>
+      <c r="G67" s="2">
         <v>0.32916666666666666</v>
       </c>
-      <c r="H46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="1">
+      <c r="H67" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" s="1">
         <v>44599</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C68" t="s">
         <v>10</v>
       </c>
-      <c r="D47">
+      <c r="D68">
         <v>207</v>
       </c>
-      <c r="E47">
+      <c r="E68">
         <v>93</v>
       </c>
-      <c r="F47">
+      <c r="F68">
         <v>32</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G68" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H47" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="1">
+      <c r="H68" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="1">
         <v>44600</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C69" t="s">
         <v>11</v>
       </c>
-      <c r="D48">
+      <c r="D69">
         <v>581</v>
       </c>
-      <c r="E48">
+      <c r="E69">
         <v>68</v>
       </c>
-      <c r="F48">
+      <c r="F69">
         <v>30</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G69" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A49" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" s="1">
+      <c r="H69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="1">
         <v>44601</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C70" t="s">
         <v>12</v>
       </c>
-      <c r="D49">
+      <c r="D70">
         <v>650</v>
       </c>
-      <c r="E49">
+      <c r="E70">
         <v>43</v>
       </c>
-      <c r="F49">
+      <c r="F70">
         <v>41</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G70" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" s="1">
+      <c r="H70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="1">
         <v>44602</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C71" t="s">
         <v>13</v>
       </c>
-      <c r="D50">
+      <c r="D71">
         <v>342</v>
       </c>
-      <c r="E50">
+      <c r="E71">
         <v>94</v>
       </c>
-      <c r="F50">
+      <c r="F71">
         <v>48</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G71" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="H50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A51" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" s="1">
+      <c r="H71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="1">
         <v>44603</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C72" t="s">
         <v>7</v>
       </c>
-      <c r="D51">
+      <c r="D72">
         <v>449</v>
       </c>
-      <c r="E51">
+      <c r="E72">
         <v>212</v>
       </c>
-      <c r="F51">
+      <c r="F72">
         <v>24</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G72" s="2">
         <v>0.30694444444444441</v>
       </c>
-      <c r="H51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" s="1">
+      <c r="H72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73" s="1">
         <v>44604</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C73" t="s">
         <v>8</v>
       </c>
-      <c r="D52">
+      <c r="D73">
         <v>497</v>
       </c>
-      <c r="E52">
+      <c r="E73">
         <v>12</v>
       </c>
-      <c r="F52">
+      <c r="F73">
         <v>28</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G73" s="2">
         <v>0.31597222222222221</v>
       </c>
-      <c r="H52" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A53" t="s">
-        <v>17</v>
-      </c>
-      <c r="B53" s="1">
+      <c r="H73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74" s="1">
         <v>44605</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C74" t="s">
         <v>9</v>
       </c>
-      <c r="D53">
+      <c r="D74">
         <v>343</v>
       </c>
-      <c r="E53">
-        <v>15</v>
-      </c>
-      <c r="F53">
+      <c r="E74">
+        <v>15</v>
+      </c>
+      <c r="F74">
         <v>38</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G74" s="2">
         <v>0.30902777777777779</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H74" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>